<commit_message>
Updated musical scale list
</commit_message>
<xml_diff>
--- a/Learning-GB-Programming/sound/musical_scale_list.xlsx
+++ b/Learning-GB-Programming/sound/musical_scale_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emutyworks-my.sharepoint.com/personal/emuty_emutyworks_onmicrosoft_com/Documents/_github/emutyworks.github.io/Learning-GB-Programming/sound/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="298" documentId="8_{AC067363-EDCD-4963-AB6F-FACFB3DEE615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C91857F-C6D4-4BA6-9387-EADD69B842E9}"/>
+  <xr:revisionPtr revIDLastSave="380" documentId="8_{AC067363-EDCD-4963-AB6F-FACFB3DEE615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18CAF866-2CFE-45FC-B484-88360AD8443D}"/>
   <bookViews>
-    <workbookView xWindow="3585" yWindow="2640" windowWidth="18360" windowHeight="12810" xr2:uid="{2AEBEDD3-01DE-4D17-AF01-4779E3A29845}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{2AEBEDD3-01DE-4D17-AF01-4779E3A29845}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -731,12 +731,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
@@ -780,7 +780,7 @@
         <v>44</v>
       </c>
       <c r="E2" s="7">
-        <f t="shared" ref="E2:E14" si="0">131072/(2048-D2)</f>
+        <f>131072/(2048-D2)</f>
         <v>65.405189620758478</v>
       </c>
       <c r="F2" s="13">
@@ -796,7 +796,7 @@
         <v>88</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B66" si="1">"%"&amp;DEC2BIN(MOD($D3,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D3,256),3)</f>
+        <f>"%"&amp;DEC2BIN(MOD($D3,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D3,256),3)</f>
         <v>%10011101,%000</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -806,14 +806,14 @@
         <v>157</v>
       </c>
       <c r="E3" s="7">
-        <f t="shared" si="0"/>
+        <f>131072/(2048-D3)</f>
         <v>69.313590692755156</v>
       </c>
       <c r="F3" s="13">
         <v>69.3</v>
       </c>
       <c r="G3" s="7">
-        <f t="shared" ref="G3:G66" si="2">F3-E3</f>
+        <f>F3-E3</f>
         <v>-1.3590692755158784E-2</v>
       </c>
     </row>
@@ -822,7 +822,7 @@
         <v>88</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D4,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D4,256),3)</f>
         <v>%00000111,%001</v>
       </c>
       <c r="C4" s="8" t="s">
@@ -832,14 +832,14 @@
         <v>263</v>
       </c>
       <c r="E4" s="7">
-        <f t="shared" si="0"/>
+        <f>131072/(2048-D4)</f>
         <v>73.429691876750695</v>
       </c>
       <c r="F4" s="13">
         <v>73.42</v>
       </c>
       <c r="G4" s="7">
-        <f t="shared" si="2"/>
+        <f>F4-E4</f>
         <v>-9.6918767506934955E-3</v>
       </c>
     </row>
@@ -848,7 +848,7 @@
         <v>88</v>
       </c>
       <c r="B5" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D5,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D5,256),3)</f>
         <v>%01101011,%001</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -858,14 +858,14 @@
         <v>363</v>
       </c>
       <c r="E5" s="7">
-        <f t="shared" si="0"/>
+        <f>131072/(2048-D5)</f>
         <v>77.787537091988128</v>
       </c>
       <c r="F5" s="13">
         <v>77.78</v>
       </c>
       <c r="G5" s="7">
-        <f t="shared" si="2"/>
+        <f>F5-E5</f>
         <v>-7.5370919881265763E-3</v>
       </c>
     </row>
@@ -874,25 +874,25 @@
         <v>88</v>
       </c>
       <c r="B6" t="str">
-        <f t="shared" si="1"/>
-        <v>%11001001,%001</v>
+        <f>"%"&amp;DEC2BIN(MOD($D6,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D6,256),3)</f>
+        <v>%11001010,%001</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="8">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="E6" s="7">
-        <f t="shared" si="0"/>
-        <v>82.383406662476432</v>
+        <f>131072/(2048-D6)</f>
+        <v>82.435220125786159</v>
       </c>
       <c r="F6" s="13">
         <v>82.41</v>
       </c>
       <c r="G6" s="7">
-        <f t="shared" si="2"/>
-        <v>2.6593337523564742E-2</v>
+        <f>F6-E6</f>
+        <v>-2.5220125786162839E-2</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -900,7 +900,7 @@
         <v>88</v>
       </c>
       <c r="B7" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D7,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D7,256),3)</f>
         <v>%00100011,%010</v>
       </c>
       <c r="C7" s="8" t="s">
@@ -910,14 +910,14 @@
         <v>547</v>
       </c>
       <c r="E7" s="7">
-        <f t="shared" si="0"/>
+        <f>131072/(2048-D7)</f>
         <v>87.323117921385744</v>
       </c>
       <c r="F7" s="13">
         <v>87.31</v>
       </c>
       <c r="G7" s="7">
-        <f t="shared" si="2"/>
+        <f>F7-E7</f>
         <v>-1.3117921385742193E-2</v>
       </c>
     </row>
@@ -926,7 +926,7 @@
         <v>88</v>
       </c>
       <c r="B8" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D8,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D8,256),3)</f>
         <v>%01110111,%010</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -936,14 +936,14 @@
         <v>631</v>
       </c>
       <c r="E8" s="7">
-        <f t="shared" si="0"/>
+        <f>131072/(2048-D8)</f>
         <v>92.499647141848982</v>
       </c>
       <c r="F8" s="13">
         <v>92.5</v>
       </c>
       <c r="G8" s="7">
-        <f t="shared" si="2"/>
+        <f>F8-E8</f>
         <v>3.5285815101815388E-4</v>
       </c>
     </row>
@@ -952,7 +952,7 @@
         <v>88</v>
       </c>
       <c r="B9" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D9,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D9,256),3)</f>
         <v>%11000111,%010</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -962,14 +962,14 @@
         <v>711</v>
       </c>
       <c r="E9" s="7">
-        <f t="shared" si="0"/>
+        <f>131072/(2048-D9)</f>
         <v>98.034405385190723</v>
       </c>
       <c r="F9" s="13">
         <v>98</v>
       </c>
       <c r="G9" s="7">
-        <f t="shared" si="2"/>
+        <f>F9-E9</f>
         <v>-3.4405385190723337E-2</v>
       </c>
     </row>
@@ -978,7 +978,7 @@
         <v>88</v>
       </c>
       <c r="B10" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D10,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D10,256),3)</f>
         <v>%00010010,%011</v>
       </c>
       <c r="C10" s="8" t="s">
@@ -988,14 +988,14 @@
         <v>786</v>
       </c>
       <c r="E10" s="7">
-        <f t="shared" si="0"/>
+        <f>131072/(2048-D10)</f>
         <v>103.86053882725832</v>
       </c>
       <c r="F10" s="13">
         <v>103.83</v>
       </c>
       <c r="G10" s="7">
-        <f t="shared" si="2"/>
+        <f>F10-E10</f>
         <v>-3.0538827258325796E-2</v>
       </c>
     </row>
@@ -1004,7 +1004,7 @@
         <v>88</v>
       </c>
       <c r="B11" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D11,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D11,256),3)</f>
         <v>%01011001,%011</v>
       </c>
       <c r="C11" s="8" t="s">
@@ -1014,14 +1014,14 @@
         <v>857</v>
       </c>
       <c r="E11" s="7">
-        <f t="shared" si="0"/>
+        <f>131072/(2048-D11)</f>
         <v>110.05205709487825</v>
       </c>
       <c r="F11" s="13">
         <v>110</v>
       </c>
       <c r="G11" s="7">
-        <f t="shared" si="2"/>
+        <f>F11-E11</f>
         <v>-5.2057094878250609E-2</v>
       </c>
     </row>
@@ -1030,7 +1030,7 @@
         <v>88</v>
       </c>
       <c r="B12" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D12,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D12,256),3)</f>
         <v>%10011011,%011</v>
       </c>
       <c r="C12" s="8" t="s">
@@ -1040,14 +1040,14 @@
         <v>923</v>
       </c>
       <c r="E12" s="7">
-        <f t="shared" si="0"/>
+        <f>131072/(2048-D12)</f>
         <v>116.50844444444445</v>
       </c>
       <c r="F12" s="13">
         <v>116.54</v>
       </c>
       <c r="G12" s="7">
-        <f t="shared" si="2"/>
+        <f>F12-E12</f>
         <v>3.1555555555556225E-2</v>
       </c>
     </row>
@@ -1056,25 +1056,25 @@
         <v>88</v>
       </c>
       <c r="B13" t="str">
-        <f t="shared" si="1"/>
-        <v>%11011010,%011</v>
+        <f>"%"&amp;DEC2BIN(MOD($D13,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D13,256),3)</f>
+        <v>%11011011,%011</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D13" s="8">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E13" s="7">
-        <f t="shared" si="0"/>
-        <v>123.41996233521657</v>
+        <f>131072/(2048-D13)</f>
+        <v>123.53628652214891</v>
       </c>
       <c r="F13" s="13">
         <v>123.47</v>
       </c>
       <c r="G13" s="7">
-        <f t="shared" si="2"/>
-        <v>5.0037664783431524E-2</v>
+        <f>F13-E13</f>
+        <v>-6.6286522148914173E-2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1082,7 +1082,7 @@
         <v>88</v>
       </c>
       <c r="B14" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D14,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D14,256),3)</f>
         <v>%00010110,%100</v>
       </c>
       <c r="C14" s="8" t="s">
@@ -1092,14 +1092,14 @@
         <v>1046</v>
       </c>
       <c r="E14" s="7">
-        <f t="shared" si="0"/>
+        <f>131072/(2048-D14)</f>
         <v>130.81037924151696</v>
       </c>
       <c r="F14" s="13">
         <v>130.81</v>
       </c>
       <c r="G14" s="7">
-        <f t="shared" si="2"/>
+        <f>F14-E14</f>
         <v>-3.7924151695278852E-4</v>
       </c>
     </row>
@@ -1108,7 +1108,7 @@
         <v>88</v>
       </c>
       <c r="B15" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D15,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D15,256),3)</f>
         <v>%01001110,%100</v>
       </c>
       <c r="C15" s="8" t="s">
@@ -1118,14 +1118,14 @@
         <v>1102</v>
       </c>
       <c r="E15" s="7">
-        <f t="shared" ref="E15:E73" si="3">131072/(2048-D15)</f>
+        <f>131072/(2048-D15)</f>
         <v>138.553911205074</v>
       </c>
       <c r="F15" s="13">
         <v>138.59</v>
       </c>
       <c r="G15" s="7">
-        <f t="shared" si="2"/>
+        <f>F15-E15</f>
         <v>3.608879492600181E-2</v>
       </c>
     </row>
@@ -1134,7 +1134,7 @@
         <v>88</v>
       </c>
       <c r="B16" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D16,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D16,256),3)</f>
         <v>%10000011,%100</v>
       </c>
       <c r="C16" s="8" t="s">
@@ -1144,14 +1144,14 @@
         <v>1155</v>
       </c>
       <c r="E16" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D16)</f>
         <v>146.77715565509519</v>
       </c>
       <c r="F16" s="13">
         <v>146.83000000000001</v>
       </c>
       <c r="G16" s="7">
-        <f t="shared" si="2"/>
+        <f>F16-E16</f>
         <v>5.2844344904826812E-2</v>
       </c>
     </row>
@@ -1160,7 +1160,7 @@
         <v>88</v>
       </c>
       <c r="B17" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D17,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D17,256),3)</f>
         <v>%10110101,%100</v>
       </c>
       <c r="C17" s="8" t="s">
@@ -1170,14 +1170,14 @@
         <v>1205</v>
       </c>
       <c r="E17" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D17)</f>
         <v>155.48279952550416</v>
       </c>
       <c r="F17" s="13">
         <v>155.56</v>
       </c>
       <c r="G17" s="7">
-        <f t="shared" si="2"/>
+        <f>F17-E17</f>
         <v>7.7200474495839444E-2</v>
       </c>
     </row>
@@ -1186,7 +1186,7 @@
         <v>88</v>
       </c>
       <c r="B18" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D18,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D18,256),3)</f>
         <v>%11100101,%100</v>
       </c>
       <c r="C18" s="8" t="s">
@@ -1196,14 +1196,14 @@
         <v>1253</v>
       </c>
       <c r="E18" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D18)</f>
         <v>164.87044025157232</v>
       </c>
       <c r="F18" s="13">
         <v>164.81</v>
       </c>
       <c r="G18" s="7">
-        <f t="shared" si="2"/>
+        <f>F18-E18</f>
         <v>-6.0440251572316583E-2</v>
       </c>
     </row>
@@ -1212,7 +1212,7 @@
         <v>88</v>
       </c>
       <c r="B19" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D19,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D19,256),3)</f>
         <v>%00010001,%101</v>
       </c>
       <c r="C19" s="8" t="s">
@@ -1222,14 +1222,14 @@
         <v>1297</v>
       </c>
       <c r="E19" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D19)</f>
         <v>174.52996005326233</v>
       </c>
       <c r="F19" s="13">
         <v>174.61</v>
       </c>
       <c r="G19" s="7">
-        <f t="shared" si="2"/>
+        <f>F19-E19</f>
         <v>8.0039946737684886E-2</v>
       </c>
     </row>
@@ -1238,7 +1238,7 @@
         <v>88</v>
       </c>
       <c r="B20" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D20,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D20,256),3)</f>
         <v>%00111011,%101</v>
       </c>
       <c r="C20" s="8" t="s">
@@ -1248,14 +1248,14 @@
         <v>1339</v>
       </c>
       <c r="E20" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D20)</f>
         <v>184.8688293370945</v>
       </c>
       <c r="F20" s="13">
         <v>185</v>
       </c>
       <c r="G20" s="7">
-        <f t="shared" si="2"/>
+        <f>F20-E20</f>
         <v>0.13117066290550383</v>
       </c>
     </row>
@@ -1264,7 +1264,7 @@
         <v>88</v>
       </c>
       <c r="B21" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D21,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D21,256),3)</f>
         <v>%01100011,%101</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -1274,14 +1274,14 @@
         <v>1379</v>
       </c>
       <c r="E21" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D21)</f>
         <v>195.92227204783259</v>
       </c>
       <c r="F21" s="13">
         <v>196</v>
       </c>
       <c r="G21" s="7">
-        <f t="shared" si="2"/>
+        <f>F21-E21</f>
         <v>7.7727952167407466E-2</v>
       </c>
     </row>
@@ -1290,7 +1290,7 @@
         <v>88</v>
       </c>
       <c r="B22" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D22,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D22,256),3)</f>
         <v>%10001001,%101</v>
       </c>
       <c r="C22" s="8" t="s">
@@ -1300,14 +1300,14 @@
         <v>1417</v>
       </c>
       <c r="E22" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D22)</f>
         <v>207.72107765451665</v>
       </c>
       <c r="F22" s="13">
         <v>207.65</v>
       </c>
       <c r="G22" s="7">
-        <f t="shared" si="2"/>
+        <f>F22-E22</f>
         <v>-7.1077654516642497E-2</v>
       </c>
     </row>
@@ -1316,7 +1316,7 @@
         <v>88</v>
       </c>
       <c r="B23" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D23,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D23,256),3)</f>
         <v>%10101100,%101</v>
       </c>
       <c r="C23" s="8" t="s">
@@ -1326,14 +1326,14 @@
         <v>1452</v>
       </c>
       <c r="E23" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D23)</f>
         <v>219.91946308724832</v>
       </c>
       <c r="F23" s="13">
         <v>220</v>
       </c>
       <c r="G23" s="7">
-        <f t="shared" si="2"/>
+        <f>F23-E23</f>
         <v>8.0536912751682621E-2</v>
       </c>
     </row>
@@ -1342,7 +1342,7 @@
         <v>88</v>
       </c>
       <c r="B24" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D24,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D24,256),3)</f>
         <v>%11001110,%101</v>
       </c>
       <c r="C24" s="8" t="s">
@@ -1352,14 +1352,14 @@
         <v>1486</v>
       </c>
       <c r="E24" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D24)</f>
         <v>233.22419928825622</v>
       </c>
       <c r="F24" s="13">
         <v>233.08</v>
       </c>
       <c r="G24" s="7">
-        <f t="shared" si="2"/>
+        <f>F24-E24</f>
         <v>-0.14419928825620332</v>
       </c>
     </row>
@@ -1368,7 +1368,7 @@
         <v>88</v>
       </c>
       <c r="B25" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D25,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D25,256),3)</f>
         <v>%11101101,%101</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -1378,14 +1378,14 @@
         <v>1517</v>
       </c>
       <c r="E25" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D25)</f>
         <v>246.83992467043313</v>
       </c>
       <c r="F25" s="13">
         <v>246.94</v>
       </c>
       <c r="G25" s="7">
-        <f t="shared" si="2"/>
+        <f>F25-E25</f>
         <v>0.10007532956686305</v>
       </c>
     </row>
@@ -1394,25 +1394,25 @@
         <v>88</v>
       </c>
       <c r="B26" t="str">
-        <f t="shared" si="1"/>
-        <v>%00001010,%110</v>
+        <f>"%"&amp;DEC2BIN(MOD($D26,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D26,256),3)</f>
+        <v>%00001011,%110</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>39</v>
       </c>
       <c r="D26" s="8">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="E26" s="7">
-        <f t="shared" si="3"/>
-        <v>261.09960159362549</v>
+        <f>131072/(2048-D26)</f>
+        <v>261.62075848303391</v>
       </c>
       <c r="F26" s="13">
         <v>261.63</v>
       </c>
       <c r="G26" s="7">
-        <f t="shared" si="2"/>
-        <v>0.53039840637450197</v>
+        <f>F26-E26</f>
+        <v>9.241516966085328E-3</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1420,7 +1420,7 @@
         <v>88</v>
       </c>
       <c r="B27" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D27,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D27,256),3)</f>
         <v>%00100111,%110</v>
       </c>
       <c r="C27" s="8" t="s">
@@ -1430,14 +1430,14 @@
         <v>1575</v>
       </c>
       <c r="E27" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D27)</f>
         <v>277.107822410148</v>
       </c>
       <c r="F27" s="13">
         <v>277.18</v>
       </c>
       <c r="G27" s="7">
-        <f t="shared" si="2"/>
+        <f>F27-E27</f>
         <v>7.2177589852003621E-2</v>
       </c>
     </row>
@@ -1446,7 +1446,7 @@
         <v>88</v>
       </c>
       <c r="B28" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D28,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D28,256),3)</f>
         <v>%01000010,%110</v>
       </c>
       <c r="C28" s="8" t="s">
@@ -1456,14 +1456,14 @@
         <v>1602</v>
       </c>
       <c r="E28" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D28)</f>
         <v>293.88340807174887</v>
       </c>
       <c r="F28" s="13">
         <v>293.66000000000003</v>
       </c>
       <c r="G28" s="7">
-        <f t="shared" si="2"/>
+        <f>F28-E28</f>
         <v>-0.22340807174884958</v>
       </c>
     </row>
@@ -1472,7 +1472,7 @@
         <v>88</v>
       </c>
       <c r="B29" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D29,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D29,256),3)</f>
         <v>%01011011,%110</v>
       </c>
       <c r="C29" s="8" t="s">
@@ -1482,14 +1482,14 @@
         <v>1627</v>
       </c>
       <c r="E29" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D29)</f>
         <v>311.33491686460809</v>
       </c>
       <c r="F29" s="13">
         <v>311.13</v>
       </c>
       <c r="G29" s="7">
-        <f t="shared" si="2"/>
+        <f>F29-E29</f>
         <v>-0.20491686460809433</v>
       </c>
     </row>
@@ -1498,7 +1498,7 @@
         <v>88</v>
       </c>
       <c r="B30" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D30,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D30,256),3)</f>
         <v>%01110010,%110</v>
       </c>
       <c r="C30" s="8" t="s">
@@ -1508,14 +1508,14 @@
         <v>1650</v>
       </c>
       <c r="E30" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D30)</f>
         <v>329.32663316582915</v>
       </c>
       <c r="F30" s="13">
         <v>329.63</v>
       </c>
       <c r="G30" s="7">
-        <f t="shared" si="2"/>
+        <f>F30-E30</f>
         <v>0.30336683417084487</v>
       </c>
     </row>
@@ -1524,7 +1524,7 @@
         <v>88</v>
       </c>
       <c r="B31" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D31,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D31,256),3)</f>
         <v>%10001001,%110</v>
       </c>
       <c r="C31" s="8" t="s">
@@ -1534,14 +1534,14 @@
         <v>1673</v>
       </c>
       <c r="E31" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D31)</f>
         <v>349.52533333333332</v>
       </c>
       <c r="F31" s="13">
         <v>349.23</v>
       </c>
       <c r="G31" s="7">
-        <f t="shared" si="2"/>
+        <f>F31-E31</f>
         <v>-0.29533333333330347</v>
       </c>
     </row>
@@ -1550,7 +1550,7 @@
         <v>88</v>
       </c>
       <c r="B32" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D32,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D32,256),3)</f>
         <v>%10011110,%110</v>
       </c>
       <c r="C32" s="8" t="s">
@@ -1560,14 +1560,14 @@
         <v>1694</v>
       </c>
       <c r="E32" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D32)</f>
         <v>370.25988700564972</v>
       </c>
       <c r="F32" s="13">
         <v>369.99</v>
       </c>
       <c r="G32" s="7">
-        <f t="shared" si="2"/>
+        <f>F32-E32</f>
         <v>-0.26988700564970713</v>
       </c>
     </row>
@@ -1576,7 +1576,7 @@
         <v>88</v>
       </c>
       <c r="B33" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D33,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D33,256),3)</f>
         <v>%10110010,%110</v>
       </c>
       <c r="C33" s="8" t="s">
@@ -1586,14 +1586,14 @@
         <v>1714</v>
       </c>
       <c r="E33" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D33)</f>
         <v>392.43113772455092</v>
       </c>
       <c r="F33" s="13">
         <v>392</v>
       </c>
       <c r="G33" s="7">
-        <f t="shared" si="2"/>
+        <f>F33-E33</f>
         <v>-0.43113772455092203</v>
       </c>
     </row>
@@ -1602,7 +1602,7 @@
         <v>88</v>
       </c>
       <c r="B34" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D34,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D34,256),3)</f>
         <v>%11000100,%110</v>
       </c>
       <c r="C34" s="8" t="s">
@@ -1612,14 +1612,14 @@
         <v>1732</v>
       </c>
       <c r="E34" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D34)</f>
         <v>414.78481012658227</v>
       </c>
       <c r="F34" s="13">
         <v>415.3</v>
       </c>
       <c r="G34" s="7">
-        <f t="shared" si="2"/>
+        <f>F34-E34</f>
         <v>0.51518987341773936</v>
       </c>
     </row>
@@ -1628,7 +1628,7 @@
         <v>88</v>
       </c>
       <c r="B35" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D35,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D35,256),3)</f>
         <v>%11010110,%110</v>
       </c>
       <c r="C35" s="8" t="s">
@@ -1638,14 +1638,14 @@
         <v>1750</v>
       </c>
       <c r="E35" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D35)</f>
         <v>439.83892617449663</v>
       </c>
       <c r="F35" s="13">
         <v>440</v>
       </c>
       <c r="G35" s="7">
-        <f t="shared" si="2"/>
+        <f>F35-E35</f>
         <v>0.16107382550336524</v>
       </c>
     </row>
@@ -1654,7 +1654,7 @@
         <v>88</v>
       </c>
       <c r="B36" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D36,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D36,256),3)</f>
         <v>%11100111,%110</v>
       </c>
       <c r="C36" s="8" t="s">
@@ -1664,14 +1664,14 @@
         <v>1767</v>
       </c>
       <c r="E36" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D36)</f>
         <v>466.44839857651243</v>
       </c>
       <c r="F36" s="13">
         <v>466.16</v>
       </c>
       <c r="G36" s="7">
-        <f t="shared" si="2"/>
+        <f>F36-E36</f>
         <v>-0.28839857651240663</v>
       </c>
     </row>
@@ -1680,7 +1680,7 @@
         <v>88</v>
       </c>
       <c r="B37" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D37,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D37,256),3)</f>
         <v>%11110111,%110</v>
       </c>
       <c r="C37" s="8" t="s">
@@ -1690,14 +1690,14 @@
         <v>1783</v>
       </c>
       <c r="E37" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D37)</f>
         <v>494.61132075471698</v>
       </c>
       <c r="F37" s="13">
         <v>493.88</v>
       </c>
       <c r="G37" s="7">
-        <f t="shared" si="2"/>
+        <f>F37-E37</f>
         <v>-0.73132075471698954</v>
       </c>
     </row>
@@ -1706,25 +1706,25 @@
         <v>88</v>
       </c>
       <c r="B38" t="str">
-        <f t="shared" si="1"/>
-        <v>%00000110,%111</v>
+        <f>"%"&amp;DEC2BIN(MOD($D38,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D38,256),3)</f>
+        <v>%00000101,%111</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>51</v>
       </c>
       <c r="D38" s="8">
-        <v>1798</v>
+        <v>1797</v>
       </c>
       <c r="E38" s="7">
-        <f t="shared" si="3"/>
-        <v>524.28800000000001</v>
+        <f>131072/(2048-D38)</f>
+        <v>522.19920318725099</v>
       </c>
       <c r="F38" s="13">
         <v>523.25</v>
       </c>
       <c r="G38" s="7">
-        <f t="shared" si="2"/>
-        <v>-1.0380000000000109</v>
+        <f>F38-E38</f>
+        <v>1.050796812749013</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1732,7 +1732,7 @@
         <v>88</v>
       </c>
       <c r="B39" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D39,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D39,256),3)</f>
         <v>%00010100,%111</v>
       </c>
       <c r="C39" s="8" t="s">
@@ -1742,14 +1742,14 @@
         <v>1812</v>
       </c>
       <c r="E39" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D39)</f>
         <v>555.38983050847457</v>
       </c>
       <c r="F39" s="13">
         <v>554.37</v>
       </c>
       <c r="G39" s="7">
-        <f t="shared" si="2"/>
+        <f>F39-E39</f>
         <v>-1.0198305084745698</v>
       </c>
     </row>
@@ -1758,7 +1758,7 @@
         <v>88</v>
       </c>
       <c r="B40" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D40,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D40,256),3)</f>
         <v>%00100001,%111</v>
       </c>
       <c r="C40" s="8" t="s">
@@ -1768,14 +1768,14 @@
         <v>1825</v>
       </c>
       <c r="E40" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D40)</f>
         <v>587.76681614349775</v>
       </c>
       <c r="F40" s="13">
         <v>587.33000000000004</v>
       </c>
       <c r="G40" s="7">
-        <f t="shared" si="2"/>
+        <f>F40-E40</f>
         <v>-0.43681614349770825</v>
       </c>
     </row>
@@ -1784,7 +1784,7 @@
         <v>88</v>
       </c>
       <c r="B41" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D41,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D41,256),3)</f>
         <v>%00101101,%111</v>
       </c>
       <c r="C41" s="8" t="s">
@@ -1794,14 +1794,14 @@
         <v>1837</v>
       </c>
       <c r="E41" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D41)</f>
         <v>621.19431279620858</v>
       </c>
       <c r="F41" s="13">
         <v>622.25</v>
       </c>
       <c r="G41" s="7">
-        <f t="shared" si="2"/>
+        <f>F41-E41</f>
         <v>1.0556872037914218</v>
       </c>
     </row>
@@ -1810,7 +1810,7 @@
         <v>88</v>
       </c>
       <c r="B42" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D42,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D42,256),3)</f>
         <v>%00111001,%111</v>
       </c>
       <c r="C42" s="8" t="s">
@@ -1820,14 +1820,14 @@
         <v>1849</v>
       </c>
       <c r="E42" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D42)</f>
         <v>658.6532663316583</v>
       </c>
       <c r="F42" s="13">
         <v>659.25</v>
       </c>
       <c r="G42" s="7">
-        <f t="shared" si="2"/>
+        <f>F42-E42</f>
         <v>0.59673366834169883</v>
       </c>
     </row>
@@ -1836,7 +1836,7 @@
         <v>88</v>
       </c>
       <c r="B43" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D43,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D43,256),3)</f>
         <v>%01000100,%111</v>
       </c>
       <c r="C43" s="8" t="s">
@@ -1846,14 +1846,14 @@
         <v>1860</v>
       </c>
       <c r="E43" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D43)</f>
         <v>697.19148936170211</v>
       </c>
       <c r="F43" s="13">
         <v>698.46</v>
       </c>
       <c r="G43" s="7">
-        <f t="shared" si="2"/>
+        <f>F43-E43</f>
         <v>1.2685106382979257</v>
       </c>
     </row>
@@ -1862,7 +1862,7 @@
         <v>88</v>
       </c>
       <c r="B44" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D44,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D44,256),3)</f>
         <v>%01001111,%111</v>
       </c>
       <c r="C44" s="8" t="s">
@@ -1872,14 +1872,14 @@
         <v>1871</v>
       </c>
       <c r="E44" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D44)</f>
         <v>740.51977401129943</v>
       </c>
       <c r="F44" s="13">
         <v>739.99</v>
       </c>
       <c r="G44" s="7">
-        <f t="shared" si="2"/>
+        <f>F44-E44</f>
         <v>-0.52977401129942336</v>
       </c>
     </row>
@@ -1888,7 +1888,7 @@
         <v>88</v>
       </c>
       <c r="B45" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D45,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D45,256),3)</f>
         <v>%01011001,%111</v>
       </c>
       <c r="C45" s="8" t="s">
@@ -1898,14 +1898,14 @@
         <v>1881</v>
       </c>
       <c r="E45" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D45)</f>
         <v>784.86227544910184</v>
       </c>
       <c r="F45" s="13">
         <v>783.99</v>
       </c>
       <c r="G45" s="7">
-        <f t="shared" si="2"/>
+        <f>F45-E45</f>
         <v>-0.87227544910183497</v>
       </c>
     </row>
@@ -1914,7 +1914,7 @@
         <v>88</v>
       </c>
       <c r="B46" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D46,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D46,256),3)</f>
         <v>%01100010,%111</v>
       </c>
       <c r="C46" s="8" t="s">
@@ -1924,14 +1924,14 @@
         <v>1890</v>
       </c>
       <c r="E46" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D46)</f>
         <v>829.56962025316454</v>
       </c>
       <c r="F46" s="13">
         <v>830.61</v>
       </c>
       <c r="G46" s="7">
-        <f t="shared" si="2"/>
+        <f>F46-E46</f>
         <v>1.0403797468354696</v>
       </c>
     </row>
@@ -1940,7 +1940,7 @@
         <v>88</v>
       </c>
       <c r="B47" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D47,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D47,256),3)</f>
         <v>%01101011,%111</v>
       </c>
       <c r="C47" s="8" t="s">
@@ -1950,14 +1950,14 @@
         <v>1899</v>
       </c>
       <c r="E47" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D47)</f>
         <v>879.67785234899327</v>
       </c>
       <c r="F47" s="13">
         <v>880</v>
       </c>
       <c r="G47" s="7">
-        <f t="shared" si="2"/>
+        <f>F47-E47</f>
         <v>0.32214765100673048</v>
       </c>
     </row>
@@ -1966,7 +1966,7 @@
         <v>88</v>
       </c>
       <c r="B48" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D48,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D48,256),3)</f>
         <v>%01110011,%111</v>
       </c>
       <c r="C48" s="8" t="s">
@@ -1976,14 +1976,14 @@
         <v>1907</v>
       </c>
       <c r="E48" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D48)</f>
         <v>929.58865248226948</v>
       </c>
       <c r="F48" s="13">
         <v>932.33</v>
       </c>
       <c r="G48" s="7">
-        <f t="shared" si="2"/>
+        <f>F48-E48</f>
         <v>2.74134751773056</v>
       </c>
     </row>
@@ -1992,7 +1992,7 @@
         <v>88</v>
       </c>
       <c r="B49" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D49,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D49,256),3)</f>
         <v>%01111011,%111</v>
       </c>
       <c r="C49" s="8" t="s">
@@ -2002,14 +2002,14 @@
         <v>1915</v>
       </c>
       <c r="E49" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D49)</f>
         <v>985.50375939849619</v>
       </c>
       <c r="F49" s="13">
         <v>987.77</v>
       </c>
       <c r="G49" s="7">
-        <f t="shared" si="2"/>
+        <f>F49-E49</f>
         <v>2.2662406015037959</v>
       </c>
     </row>
@@ -2018,7 +2018,7 @@
         <v>88</v>
       </c>
       <c r="B50" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D50,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D50,256),3)</f>
         <v>%10000011,%111</v>
       </c>
       <c r="C50" s="8" t="s">
@@ -2028,14 +2028,14 @@
         <v>1923</v>
       </c>
       <c r="E50" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D50)</f>
         <v>1048.576</v>
       </c>
       <c r="F50" s="13">
         <v>1046.5</v>
       </c>
       <c r="G50" s="7">
-        <f t="shared" si="2"/>
+        <f>F50-E50</f>
         <v>-2.0760000000000218</v>
       </c>
     </row>
@@ -2044,7 +2044,7 @@
         <v>88</v>
       </c>
       <c r="B51" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D51,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D51,256),3)</f>
         <v>%10001010,%111</v>
       </c>
       <c r="C51" s="8" t="s">
@@ -2054,14 +2054,14 @@
         <v>1930</v>
       </c>
       <c r="E51" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D51)</f>
         <v>1110.7796610169491</v>
       </c>
       <c r="F51" s="13">
         <v>1108.73</v>
       </c>
       <c r="G51" s="7">
-        <f t="shared" si="2"/>
+        <f>F51-E51</f>
         <v>-2.0496610169491305</v>
       </c>
     </row>
@@ -2070,7 +2070,7 @@
         <v>88</v>
       </c>
       <c r="B52" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D52,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D52,256),3)</f>
         <v>%10010000,%111</v>
       </c>
       <c r="C52" s="8" t="s">
@@ -2080,14 +2080,14 @@
         <v>1936</v>
       </c>
       <c r="E52" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D52)</f>
         <v>1170.2857142857142</v>
       </c>
       <c r="F52" s="13">
         <v>1174.6600000000001</v>
       </c>
       <c r="G52" s="7">
-        <f t="shared" si="2"/>
+        <f>F52-E52</f>
         <v>4.3742857142858611</v>
       </c>
     </row>
@@ -2096,7 +2096,7 @@
         <v>88</v>
       </c>
       <c r="B53" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D53,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D53,256),3)</f>
         <v>%10010111,%111</v>
       </c>
       <c r="C53" s="8" t="s">
@@ -2106,14 +2106,14 @@
         <v>1943</v>
       </c>
       <c r="E53" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D53)</f>
         <v>1248.304761904762</v>
       </c>
       <c r="F53" s="13">
         <v>1244.51</v>
       </c>
       <c r="G53" s="7">
-        <f t="shared" si="2"/>
+        <f>F53-E53</f>
         <v>-3.7947619047620265</v>
       </c>
     </row>
@@ -2122,7 +2122,7 @@
         <v>88</v>
       </c>
       <c r="B54" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D54,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D54,256),3)</f>
         <v>%10011101,%111</v>
       </c>
       <c r="C54" s="8" t="s">
@@ -2132,14 +2132,14 @@
         <v>1949</v>
       </c>
       <c r="E54" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D54)</f>
         <v>1323.9595959595961</v>
       </c>
       <c r="F54" s="13">
         <v>1318.51</v>
       </c>
       <c r="G54" s="7">
-        <f t="shared" si="2"/>
+        <f>F54-E54</f>
         <v>-5.4495959595960812</v>
       </c>
     </row>
@@ -2148,7 +2148,7 @@
         <v>88</v>
       </c>
       <c r="B55" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D55,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D55,256),3)</f>
         <v>%10100010,%111</v>
       </c>
       <c r="C55" s="8" t="s">
@@ -2158,14 +2158,14 @@
         <v>1954</v>
       </c>
       <c r="E55" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D55)</f>
         <v>1394.3829787234042</v>
       </c>
       <c r="F55" s="13">
         <v>1396.91</v>
       </c>
       <c r="G55" s="7">
-        <f t="shared" si="2"/>
+        <f>F55-E55</f>
         <v>2.5270212765958604</v>
       </c>
     </row>
@@ -2174,7 +2174,7 @@
         <v>88</v>
       </c>
       <c r="B56" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D56,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D56,256),3)</f>
         <v>%10100111,%111</v>
       </c>
       <c r="C56" s="8" t="s">
@@ -2184,14 +2184,14 @@
         <v>1959</v>
       </c>
       <c r="E56" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D56)</f>
         <v>1472.7191011235955</v>
       </c>
       <c r="F56" s="13">
         <v>1479.98</v>
       </c>
       <c r="G56" s="7">
-        <f t="shared" si="2"/>
+        <f>F56-E56</f>
         <v>7.2608988764045534</v>
       </c>
     </row>
@@ -2200,7 +2200,7 @@
         <v>88</v>
       </c>
       <c r="B57" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D57,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D57,256),3)</f>
         <v>%10101100,%111</v>
       </c>
       <c r="C57" s="8" t="s">
@@ -2210,14 +2210,14 @@
         <v>1964</v>
       </c>
       <c r="E57" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D57)</f>
         <v>1560.3809523809523</v>
       </c>
       <c r="F57" s="13">
         <v>1567.98</v>
       </c>
       <c r="G57" s="7">
-        <f t="shared" si="2"/>
+        <f>F57-E57</f>
         <v>7.5990476190477239</v>
       </c>
     </row>
@@ -2226,7 +2226,7 @@
         <v>88</v>
       </c>
       <c r="B58" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D58,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D58,256),3)</f>
         <v>%10110001,%111</v>
       </c>
       <c r="C58" s="8" t="s">
@@ -2236,14 +2236,14 @@
         <v>1969</v>
       </c>
       <c r="E58" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D58)</f>
         <v>1659.1392405063291</v>
       </c>
       <c r="F58" s="13">
         <v>1661.22</v>
       </c>
       <c r="G58" s="7">
-        <f t="shared" si="2"/>
+        <f>F58-E58</f>
         <v>2.0807594936709393</v>
       </c>
     </row>
@@ -2252,7 +2252,7 @@
         <v>88</v>
       </c>
       <c r="B59" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D59,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D59,256),3)</f>
         <v>%10110110,%111</v>
       </c>
       <c r="C59" s="8" t="s">
@@ -2262,14 +2262,14 @@
         <v>1974</v>
       </c>
       <c r="E59" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D59)</f>
         <v>1771.2432432432433</v>
       </c>
       <c r="F59" s="13">
         <v>1760</v>
       </c>
       <c r="G59" s="7">
-        <f t="shared" si="2"/>
+        <f>F59-E59</f>
         <v>-11.243243243243342</v>
       </c>
     </row>
@@ -2278,7 +2278,7 @@
         <v>88</v>
       </c>
       <c r="B60" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D60,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D60,256),3)</f>
         <v>%10111010,%111</v>
       </c>
       <c r="C60" s="8" t="s">
@@ -2288,14 +2288,14 @@
         <v>1978</v>
       </c>
       <c r="E60" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D60)</f>
         <v>1872.4571428571428</v>
       </c>
       <c r="F60" s="13">
         <v>1864.66</v>
       </c>
       <c r="G60" s="7">
-        <f t="shared" si="2"/>
+        <f>F60-E60</f>
         <v>-7.7971428571427168</v>
       </c>
     </row>
@@ -2304,7 +2304,7 @@
         <v>88</v>
       </c>
       <c r="B61" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D61,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D61,256),3)</f>
         <v>%10111110,%111</v>
       </c>
       <c r="C61" s="8" t="s">
@@ -2314,14 +2314,14 @@
         <v>1982</v>
       </c>
       <c r="E61" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D61)</f>
         <v>1985.939393939394</v>
       </c>
       <c r="F61" s="13">
         <v>1975.53</v>
       </c>
       <c r="G61" s="7">
-        <f t="shared" si="2"/>
+        <f>F61-E61</f>
         <v>-10.409393939394022</v>
       </c>
     </row>
@@ -2330,7 +2330,7 @@
         <v>88</v>
       </c>
       <c r="B62" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D62,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D62,256),3)</f>
         <v>%11000001,%111</v>
       </c>
       <c r="C62" s="8" t="s">
@@ -2340,14 +2340,14 @@
         <v>1985</v>
       </c>
       <c r="E62" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D62)</f>
         <v>2080.5079365079364</v>
       </c>
       <c r="F62" s="13">
         <v>2093</v>
       </c>
       <c r="G62" s="7">
-        <f t="shared" si="2"/>
+        <f>F62-E62</f>
         <v>12.492063492063608</v>
       </c>
     </row>
@@ -2356,25 +2356,25 @@
         <v>88</v>
       </c>
       <c r="B63" t="str">
-        <f t="shared" si="1"/>
-        <v>%11000100,%111</v>
+        <f>"%"&amp;DEC2BIN(MOD($D63,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D63,256),3)</f>
+        <v>%11000101,%111</v>
       </c>
       <c r="C63" s="8" t="s">
         <v>76</v>
       </c>
       <c r="D63" s="8">
-        <v>1988</v>
+        <v>1989</v>
       </c>
       <c r="E63" s="7">
-        <f t="shared" si="3"/>
-        <v>2184.5333333333333</v>
+        <f>131072/(2048-D63)</f>
+        <v>2221.5593220338983</v>
       </c>
       <c r="F63" s="13">
         <v>2217.46</v>
       </c>
       <c r="G63" s="7">
-        <f t="shared" si="2"/>
-        <v>32.926666666666733</v>
+        <f>F63-E63</f>
+        <v>-4.099322033898261</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -2382,7 +2382,7 @@
         <v>88</v>
       </c>
       <c r="B64" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D64,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D64,256),3)</f>
         <v>%11001000,%111</v>
       </c>
       <c r="C64" s="8" t="s">
@@ -2392,14 +2392,14 @@
         <v>1992</v>
       </c>
       <c r="E64" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D64)</f>
         <v>2340.5714285714284</v>
       </c>
       <c r="F64" s="13">
         <v>2349.3200000000002</v>
       </c>
       <c r="G64" s="7">
-        <f t="shared" si="2"/>
+        <f>F64-E64</f>
         <v>8.7485714285717222</v>
       </c>
     </row>
@@ -2408,7 +2408,7 @@
         <v>88</v>
       </c>
       <c r="B65" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D65,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D65,256),3)</f>
         <v>%11001011,%111</v>
       </c>
       <c r="C65" s="8" t="s">
@@ -2418,14 +2418,14 @@
         <v>1995</v>
       </c>
       <c r="E65" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D65)</f>
         <v>2473.0566037735848</v>
       </c>
       <c r="F65" s="13">
         <v>2489.02</v>
       </c>
       <c r="G65" s="7">
-        <f t="shared" si="2"/>
+        <f>F65-E65</f>
         <v>15.963396226415171</v>
       </c>
     </row>
@@ -2434,7 +2434,7 @@
         <v>88</v>
       </c>
       <c r="B66" t="str">
-        <f t="shared" si="1"/>
+        <f>"%"&amp;DEC2BIN(MOD($D66,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D66,256),3)</f>
         <v>%11001110,%111</v>
       </c>
       <c r="C66" s="8" t="s">
@@ -2444,14 +2444,14 @@
         <v>1998</v>
       </c>
       <c r="E66" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D66)</f>
         <v>2621.44</v>
       </c>
       <c r="F66" s="13">
         <v>2637.02</v>
       </c>
       <c r="G66" s="7">
-        <f t="shared" si="2"/>
+        <f>F66-E66</f>
         <v>15.579999999999927</v>
       </c>
     </row>
@@ -2460,7 +2460,7 @@
         <v>88</v>
       </c>
       <c r="B67" t="str">
-        <f t="shared" ref="B67:B73" si="4">"%"&amp;DEC2BIN(MOD($D67,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D67,256),3)</f>
+        <f>"%"&amp;DEC2BIN(MOD($D67,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D67,256),3)</f>
         <v>%11010001,%111</v>
       </c>
       <c r="C67" s="8" t="s">
@@ -2470,14 +2470,14 @@
         <v>2001</v>
       </c>
       <c r="E67" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D67)</f>
         <v>2788.7659574468084</v>
       </c>
       <c r="F67" s="13">
         <v>2793.83</v>
       </c>
       <c r="G67" s="7">
-        <f t="shared" ref="G67:G73" si="5">F67-E67</f>
+        <f>F67-E67</f>
         <v>5.0640425531914843</v>
       </c>
     </row>
@@ -2486,7 +2486,7 @@
         <v>88</v>
       </c>
       <c r="B68" t="str">
-        <f t="shared" si="4"/>
+        <f>"%"&amp;DEC2BIN(MOD($D68,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D68,256),3)</f>
         <v>%11010100,%111</v>
       </c>
       <c r="C68" s="8" t="s">
@@ -2496,14 +2496,14 @@
         <v>2004</v>
       </c>
       <c r="E68" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D68)</f>
         <v>2978.909090909091</v>
       </c>
       <c r="F68" s="13">
         <v>2959.96</v>
       </c>
       <c r="G68" s="7">
-        <f t="shared" si="5"/>
+        <f>F68-E68</f>
         <v>-18.949090909090955</v>
       </c>
     </row>
@@ -2512,7 +2512,7 @@
         <v>88</v>
       </c>
       <c r="B69" t="str">
-        <f t="shared" si="4"/>
+        <f>"%"&amp;DEC2BIN(MOD($D69,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D69,256),3)</f>
         <v>%11010110,%111</v>
       </c>
       <c r="C69" s="8" t="s">
@@ -2522,14 +2522,14 @@
         <v>2006</v>
       </c>
       <c r="E69" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D69)</f>
         <v>3120.7619047619046</v>
       </c>
       <c r="F69" s="13">
         <v>3135.96</v>
       </c>
       <c r="G69" s="7">
-        <f t="shared" si="5"/>
+        <f>F69-E69</f>
         <v>15.198095238095448</v>
       </c>
     </row>
@@ -2538,7 +2538,7 @@
         <v>88</v>
       </c>
       <c r="B70" t="str">
-        <f t="shared" si="4"/>
+        <f>"%"&amp;DEC2BIN(MOD($D70,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D70,256),3)</f>
         <v>%11011001,%111</v>
       </c>
       <c r="C70" s="8" t="s">
@@ -2548,14 +2548,14 @@
         <v>2009</v>
       </c>
       <c r="E70" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D70)</f>
         <v>3360.8205128205127</v>
       </c>
       <c r="F70" s="13">
         <v>3322.44</v>
       </c>
       <c r="G70" s="7">
-        <f t="shared" si="5"/>
+        <f>F70-E70</f>
         <v>-38.380512820512649</v>
       </c>
     </row>
@@ -2564,7 +2564,7 @@
         <v>88</v>
       </c>
       <c r="B71" t="str">
-        <f t="shared" si="4"/>
+        <f>"%"&amp;DEC2BIN(MOD($D71,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D71,256),3)</f>
         <v>%11011011,%111</v>
       </c>
       <c r="C71" s="8" t="s">
@@ -2574,14 +2574,14 @@
         <v>2011</v>
       </c>
       <c r="E71" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D71)</f>
         <v>3542.4864864864867</v>
       </c>
       <c r="F71" s="13">
         <v>3520</v>
       </c>
       <c r="G71" s="7">
-        <f t="shared" si="5"/>
+        <f>F71-E71</f>
         <v>-22.486486486486683</v>
       </c>
     </row>
@@ -2590,7 +2590,7 @@
         <v>88</v>
       </c>
       <c r="B72" t="str">
-        <f t="shared" si="4"/>
+        <f>"%"&amp;DEC2BIN(MOD($D72,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D72,256),3)</f>
         <v>%11011101,%111</v>
       </c>
       <c r="C72" s="8" t="s">
@@ -2600,14 +2600,14 @@
         <v>2013</v>
       </c>
       <c r="E72" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D72)</f>
         <v>3744.9142857142856</v>
       </c>
       <c r="F72" s="13">
         <v>3729.31</v>
       </c>
       <c r="G72" s="7">
-        <f t="shared" si="5"/>
+        <f>F72-E72</f>
         <v>-15.604285714285652</v>
       </c>
     </row>
@@ -2616,7 +2616,7 @@
         <v>88</v>
       </c>
       <c r="B73" t="str">
-        <f t="shared" si="4"/>
+        <f>"%"&amp;DEC2BIN(MOD($D73,256),8)&amp;",%"&amp;DEC2BIN(QUOTIENT($D73,256),3)</f>
         <v>%11011111,%111</v>
       </c>
       <c r="C73" s="8" t="s">
@@ -2626,14 +2626,14 @@
         <v>2015</v>
       </c>
       <c r="E73" s="7">
-        <f t="shared" si="3"/>
+        <f>131072/(2048-D73)</f>
         <v>3971.878787878788</v>
       </c>
       <c r="F73" s="13">
         <v>3951.07</v>
       </c>
       <c r="G73" s="7">
-        <f t="shared" si="5"/>
+        <f>F73-E73</f>
         <v>-20.808787878787825</v>
       </c>
     </row>

</xml_diff>